<commit_message>
Updated metadata file to include CO2_log_exp1.csv metadata, created CO2_log_exp1.csv
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OliviaBernauer/Documents/Research/oliviabernauer/eCO2_SciReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9971D007-D4E8-CA4C-9989-2784FBF36E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD390AD-39EE-B04B-BB4B-3BE53E1CE4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47000" yWindow="2880" windowWidth="25240" windowHeight="13940" xr2:uid="{3AAB57C8-B0D8-9F44-A9EE-DEC92E23882B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Bernauer-etal-Elevated_atmospheric_CO2_has_inconsistent_effects_on_pollen_chemistry_and_plant_growth_across_flowering_plant_species</t>
   </si>
@@ -102,6 +102,45 @@
   </si>
   <si>
     <t>If a value was an outlier, this column is blank. Outliers are calculated in CO2_plotting.R</t>
+  </si>
+  <si>
+    <t>Column descriptions for "CO2_log_exp1.csv"</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>co2_a</t>
+  </si>
+  <si>
+    <t>temp_a</t>
+  </si>
+  <si>
+    <t>datenum</t>
+  </si>
+  <si>
+    <t>Time stamp for CO2 reading in the format YYMMDD_HHMMSS</t>
+  </si>
+  <si>
+    <t>CO2 ppm reading from Licor 8500 in ambient CO2 greenhouse</t>
+  </si>
+  <si>
+    <t>CO2 ppm reading from Licor 8500 in elevated CO2 greenhouse</t>
+  </si>
+  <si>
+    <t>Temperature reading from Licor 8500 in ambient CO2 greenhouse</t>
+  </si>
+  <si>
+    <t>Temperature reading from Licor 8500 in elevated CO2 greenhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lubridate value for time stamp in "time" column used for plotting in R </t>
+  </si>
+  <si>
+    <t>co2_e</t>
+  </si>
+  <si>
+    <t>temp_e</t>
   </si>
 </sst>
 </file>
@@ -462,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F01E80B-B996-E649-A948-07229D80A5C9}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,6 +602,59 @@
         <v>21</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Flowering initiation data, updated metadata
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OliviaBernauer/Documents/Research/oliviabernauer/eCO2_SciReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB9D920-F7DC-F242-ABBA-887BD934FEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD7101A-4A68-964E-8822-D2267B1C553E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47000" yWindow="2880" windowWidth="25240" windowHeight="13940" xr2:uid="{3AAB57C8-B0D8-9F44-A9EE-DEC92E23882B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="125">
   <si>
     <t>Bernauer-etal-Elevated_atmospheric_CO2_has_inconsistent_effects_on_pollen_chemistry_and_plant_growth_across_flowering_plant_species</t>
   </si>
@@ -68,6 +68,9 @@
     <t>aco2</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Date_Time</t>
   </si>
   <si>
@@ -399,6 +402,15 @@
   </si>
   <si>
     <t>Mean flower diameter in mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column descriptions for "Flowering_initiation_exp2.csv" </t>
+  </si>
+  <si>
+    <t>Plant_ID</t>
+  </si>
+  <si>
+    <t>Date that flowering initiated</t>
   </si>
 </sst>
 </file>
@@ -769,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F01E80B-B996-E649-A948-07229D80A5C9}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,55 +815,55 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -864,7 +876,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -872,7 +884,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -880,382 +892,382 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1263,44 +1275,44 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1308,28 +1320,28 @@
         <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B76" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B77" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1337,47 +1349,100 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B81" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>123</v>
+      </c>
+      <c r="B93" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Plant_growth_exp2 and Metadata files
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OliviaBernauer/Documents/Research/oliviabernauer/eCO2_SciReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD7101A-4A68-964E-8822-D2267B1C553E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC570AD-476C-944D-B0FF-4C8BC8090511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47000" yWindow="2880" windowWidth="25240" windowHeight="13940" xr2:uid="{3AAB57C8-B0D8-9F44-A9EE-DEC92E23882B}"/>
+    <workbookView xWindow="18420" yWindow="760" windowWidth="25240" windowHeight="13940" xr2:uid="{3AAB57C8-B0D8-9F44-A9EE-DEC92E23882B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="135">
   <si>
     <t>Bernauer-etal-Elevated_atmospheric_CO2_has_inconsistent_effects_on_pollen_chemistry_and_plant_growth_across_flowering_plant_species</t>
   </si>
@@ -411,6 +411,36 @@
   </si>
   <si>
     <t>Date that flowering initiated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column descriptions for "Plant_growth_exp2.csv" </t>
+  </si>
+  <si>
+    <t>Leaf_no</t>
+  </si>
+  <si>
+    <t>Flower_no</t>
+  </si>
+  <si>
+    <t>Height_cm</t>
+  </si>
+  <si>
+    <t>Date that plant growth data was collected</t>
+  </si>
+  <si>
+    <t>Unique identifier for the individual plant where the data came from</t>
+  </si>
+  <si>
+    <t>Number of leaves (count data) on that plant on that day, measured once per week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of flowers (count data) open on that plant on that day, measured daily once flowering initiated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height of the plant from dirt to top in cm, measured once weekly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes about the plant or about data collection from that day. </t>
   </si>
 </sst>
 </file>
@@ -461,12 +491,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F01E80B-B996-E649-A948-07229D80A5C9}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,7 +1476,104 @@
         <v>70</v>
       </c>
     </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>123</v>
+      </c>
+      <c r="B100" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>126</v>
+      </c>
+      <c r="B101" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>127</v>
+      </c>
+      <c r="B102" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>128</v>
+      </c>
+      <c r="B103" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>89</v>
+      </c>
+      <c r="B104" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF7030A0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated pollen_chemistry_exp2 file and metadata file correspondingly
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OliviaBernauer/Documents/Research/oliviabernauer/eCO2_SciReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBFFC82-6AE5-9A45-BB63-5C997AB486F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36065DF-2F1E-7946-B2FE-6106B7F470BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="760" windowWidth="25240" windowHeight="13940" xr2:uid="{3AAB57C8-B0D8-9F44-A9EE-DEC92E23882B}"/>
+    <workbookView xWindow="9320" yWindow="760" windowWidth="25240" windowHeight="13940" xr2:uid="{3AAB57C8-B0D8-9F44-A9EE-DEC92E23882B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="132">
   <si>
     <t>Bernauer-etal-Elevated_atmospheric_CO2_has_inconsistent_effects_on_pollen_chemistry_and_plant_growth_across_flowering_plant_species</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Sample ID</t>
   </si>
   <si>
-    <t>Sample_weight</t>
-  </si>
-  <si>
     <t>OMIT</t>
   </si>
   <si>
@@ -353,19 +350,10 @@
     <t>Plant_SP</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Weight (in g) of pollen analyzed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Samples marked "1" were omitted from analyses due to insufficient N detected in the pollen samples as indicated in the notes column, or due to being a duplicate sample </t>
   </si>
   <si>
     <t>Plant species common name abbreviation (B = borage, BW = buckwheat, C = red clover, N = nasturtium, LP = lacy phacelia, PP, = partridge pea, SF = sunflower, SA = sweet alyssum)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual plant ID number. </t>
   </si>
   <si>
     <t>Plant ID</t>
@@ -815,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F01E80B-B996-E649-A948-07229D80A5C9}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1168,7 +1156,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1237,7 +1225,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1250,26 +1238,26 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -1277,7 +1265,7 @@
         <v>102</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1285,57 +1273,57 @@
         <v>103</v>
       </c>
       <c r="B65" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>94</v>
-      </c>
-      <c r="B69" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>61</v>
-      </c>
-      <c r="B70" t="s">
-        <v>95</v>
+      <c r="A70" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>115</v>
+      <c r="A72" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B73" t="s">
         <v>112</v>
@@ -1343,185 +1331,185 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>6</v>
       </c>
-      <c r="B75" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>94</v>
       </c>
-      <c r="B76" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>111</v>
-      </c>
-      <c r="B77" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>120</v>
+      <c r="B79" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B80" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="B81" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>115</v>
+      </c>
+      <c r="B83" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B83" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>119</v>
-      </c>
-      <c r="B85" t="s">
-        <v>121</v>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>122</v>
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B89" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>88</v>
-      </c>
-      <c r="B92" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>123</v>
-      </c>
-      <c r="B93" t="s">
-        <v>70</v>
+      <c r="A93" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>125</v>
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>10</v>
+      <c r="A96" t="s">
+        <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B97" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B98" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1529,43 +1517,27 @@
         <v>123</v>
       </c>
       <c r="B101" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B102" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B103" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>128</v>
-      </c>
-      <c r="B104" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>89</v>
-      </c>
-      <c r="B105" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A97:A98">
+  <conditionalFormatting sqref="A95:A96">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>